<commit_message>
More process scripts, results
</commit_message>
<xml_diff>
--- a/keyness.xlsx
+++ b/keyness.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="keywords.csv" sheetId="1" r:id="rId1"/>
     <sheet name="keyness and frequency" sheetId="2" r:id="rId2"/>
+    <sheet name="keyness" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -428,7 +429,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1000,11 +1000,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2103576392"/>
-        <c:axId val="2103506520"/>
+        <c:axId val="2069841144"/>
+        <c:axId val="2069844120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2103576392"/>
+        <c:axId val="2069841144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1014,7 +1014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103506520"/>
+        <c:crossAx val="2069844120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1022,7 +1022,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2103506520"/>
+        <c:axId val="2069844120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1033,7 +1033,870 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103576392"/>
+        <c:crossAx val="2069841144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>keyness</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>keywords.csv!$D$2:$D$126</c:f>
+              <c:strCache>
+                <c:ptCount val="125"/>
+                <c:pt idx="0">
+                  <c:v>monsieur</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>etat</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>veux</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>nicolas</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>euro</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>projet</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>hollande</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>français</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>marchés</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>réalité</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>madame</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>protectionnisme</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>effectivement</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>choix</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>copé</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>caste</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>hein</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>pouvoir</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>vision</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>aphatie</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>argent</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>œuvre</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>france</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>banques</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>peuple</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>austérité</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>réindustrialisation</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>grèce</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>excusez-moi</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>voilà</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>sarkozy</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>oubliés</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>rien</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>chers</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>système</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>déloyale</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>ultralibérale</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>notamment</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>pmi</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>mettre</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>permettez-moi</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>libye</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>françois</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>umps</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>groupes</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>train</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>mondialisation</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>débat</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>moyennes</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>démocratie</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>dette</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>mélenchon</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>strauss-kahn</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>pense</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>monnaie</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>élites</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>qatar</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>voyez</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>baisse</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>ultralibéralisme</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>niche</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>économique</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>amis</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>liberté</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>rassemblement</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>bonjour</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>comprenez</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>classes</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>fondamentalistes</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>sûre</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>réformes</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>parlement</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>actuellement</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>professionnelle</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>population</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>vingt</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>armée</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>doute</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>nord</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>retraite</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>politiciens</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>préférence</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>maastricht</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>électorale</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>revenu</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>agriculture</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>quatre</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>états</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>éducation</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>parait</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>trois</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>immigrés</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>mort</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>environnement</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>algérie</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>gouvernements</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>voix</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>bayrou</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>autrement</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>formation</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>guerre</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>chez</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>communiste</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>paysans</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>dois</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>deuxième</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>europe</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>ecoutez</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>national</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>pen</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>conséquent</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>hommes</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>gens</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>paris</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>particulier</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>front</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>bureau</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>jospin</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>mesdames</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>messieurs</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>jacques</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>effet</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>millions</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>ans</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>chirac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>keywords.csv!$C$2:$C$126</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="125"/>
+                <c:pt idx="0">
+                  <c:v>272.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>238.45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>238.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>197.12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>151.31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>121.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>117.77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>105.04</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>97.87</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>96.15000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>91.24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>87.15000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>85.31</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>76.79</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75.94</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>74.66</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>71.89</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>69.1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>66.11</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>65.64</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>62.91</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>62.52</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>62.09</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>61.97</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>56.79</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>55.35</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>53.27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>47.97</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45.61</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43.49</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43.16</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>42.31</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41.89</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>41.71</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40.67</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>39.9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37.75</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>37.2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>36.27</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>36.21</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>36.04</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>35.05</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>35.03</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>34.61</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>34.59</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>34.28</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>33.37</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>33.36</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>33.16</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>32.76</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>32.18</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>31.3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>31.21</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>30.63</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>29.89</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>29.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>29.35</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>28.6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>28.32</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>28.32</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>27.75</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>27.69</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>27.19</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>26.27</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>25.74</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>25.74</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>25.55</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>24.45</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>24.08</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-24.44</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-24.48</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-24.59</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-24.59</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-24.66</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-24.83</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-24.87</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-25.48</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-25.64</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-26.65</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-26.76</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-26.81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-26.94</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-27.06</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-27.25</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-27.38</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-27.68</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-28.13</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-28.64</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-28.89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-29.63</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-30.61</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-30.61</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-30.93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-31.1</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-31.3</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-32.85</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-33.42</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-34.09</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-35.68</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-36.0</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-36.55</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-36.67</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-37.24</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-37.81</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>-38.74</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-38.91</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>-39.67</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>-40.08</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>-40.15</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>-40.19</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>-40.89</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>-42.12</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>-42.22</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>-42.31</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>-43.48</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>-51.06</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>-58.89</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>-59.99</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>-63.48</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>-83.79</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>-92.11</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>-93.83</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>-97.66</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>-250.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2146494136"/>
+        <c:axId val="2146496408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2146494136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2146496408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2146496408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2146494136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1076,6 +1939,41 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1416,8 +2314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H126"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D1" activeCellId="3" sqref="C1:C1048576 A1 A1:A1048576 D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4457,6 +5355,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>